<commit_message>
Revert "Revert "Revert "Yes"""
This reverts commit bf1342e6f9a637a132f1f6165cc2ec4733cbf4e1.
</commit_message>
<xml_diff>
--- a/SUS_INTUI_WORD.xlsx
+++ b/SUS_INTUI_WORD.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\test1\Documents\P8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marianne\Desktop\P8-Analyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682AE9FC-79D2-4099-905A-5750131E54F9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11550" windowHeight="7590" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11556" windowHeight="7596" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="SusHelix" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
     <sheet name="WordHelix" sheetId="5" r:id="rId7"/>
     <sheet name="WordHeadrush" sheetId="6" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="140">
   <si>
     <t>Helix</t>
   </si>
@@ -452,15 +451,12 @@
   </si>
   <si>
     <t>ID</t>
-  </si>
-  <si>
-    <t>Comprehensiv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -514,7 +510,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Procent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -537,7 +533,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="da-DK"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -574,7 +570,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="da-DK"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1330,7 +1326,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="449834784"/>
@@ -1389,7 +1385,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="449834128"/>
@@ -1431,7 +1427,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="da-DK"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1461,7 +1457,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="da-DK"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2070,9 +2066,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kontor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2110,7 +2106,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kontor">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2216,7 +2212,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kontor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2365,20 +2361,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.21875" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2407,7 +2403,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2436,7 +2432,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2465,7 +2461,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2494,7 +2490,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2523,7 +2519,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2552,7 +2548,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2581,7 +2577,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2610,7 +2606,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2639,7 +2635,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2668,7 +2664,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2697,7 +2693,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13">
         <f>(((B2-1)+(5-B3)+(B4-1)+(5-B5)+(B6-1)+(5-B7)+(B8-1)+(5-B9)+(B10-1)+(5-B11))*2.5)</f>
         <v>60</v>
@@ -2741,16 +2737,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView topLeftCell="B7" workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -2782,7 +2778,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2815,7 +2811,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2848,7 +2844,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2881,7 +2877,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2914,7 +2910,7 @@
         <v>2.375</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2947,7 +2943,7 @@
         <v>3.625</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2980,7 +2976,7 @@
         <v>2.125</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3013,7 +3009,7 @@
         <v>3.875</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3046,7 +3042,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3079,7 +3075,7 @@
         <v>3.375</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3112,7 +3108,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13">
         <f>(((B2-1)+(5-B3)+(B4-1)+(5-B5)+(B6-1)+(5-B7)+(B8-1)+(5-B9)+(B10-1)+(5-B11))*2.5)</f>
         <v>75</v>
@@ -3157,16 +3153,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J18" sqref="A1:J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3195,7 +3191,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3227,7 +3223,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3259,7 +3255,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3291,7 +3287,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3323,7 +3319,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3355,7 +3351,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3387,7 +3383,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3419,7 +3415,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3451,7 +3447,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3483,7 +3479,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3519,7 +3515,7 @@
         <v>3.375</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3551,7 +3547,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3583,7 +3579,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3615,7 +3611,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3647,7 +3643,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3679,7 +3675,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3711,7 +3707,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3743,7 +3739,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -3785,10 +3781,10 @@
       </c>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -3830,10 +3826,10 @@
       </c>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -3875,10 +3871,10 @@
       </c>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -3920,10 +3916,10 @@
       </c>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -3971,16 +3967,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J18" sqref="A1:J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -4009,7 +4005,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4041,7 +4037,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4073,7 +4069,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4108,7 +4104,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4140,7 +4136,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4172,7 +4168,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4207,7 +4203,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4239,7 +4235,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4274,7 +4270,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4309,7 +4305,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4345,7 +4341,7 @@
         <v>4.125</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4377,7 +4373,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4409,7 +4405,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4444,7 +4440,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4479,7 +4475,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4511,7 +4507,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4546,7 +4542,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4578,7 +4574,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -4620,10 +4616,10 @@
       </c>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -4665,10 +4661,10 @@
       </c>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -4710,10 +4706,10 @@
       </c>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -4755,10 +4751,10 @@
       </c>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -4806,16 +4802,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -4847,7 +4843,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -4879,7 +4875,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>5</v>
       </c>
@@ -4911,7 +4907,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>7</v>
       </c>
@@ -4943,7 +4939,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>9</v>
       </c>
@@ -4975,7 +4971,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>13</v>
       </c>
@@ -5007,7 +5003,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -5039,7 +5035,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3</v>
       </c>
@@ -5071,7 +5067,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>4</v>
       </c>
@@ -5103,7 +5099,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>6</v>
       </c>
@@ -5135,7 +5131,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>11</v>
       </c>
@@ -5167,7 +5163,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>15</v>
       </c>
@@ -5199,7 +5195,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>16</v>
       </c>
@@ -5231,7 +5227,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>17</v>
       </c>
@@ -5263,7 +5259,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>8</v>
       </c>
@@ -5295,7 +5291,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>10</v>
       </c>
@@ -5327,7 +5323,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>12</v>
       </c>
@@ -5359,7 +5355,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>14</v>
       </c>
@@ -5400,16 +5396,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M41" sqref="M41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5441,7 +5437,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -5473,7 +5469,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>5</v>
       </c>
@@ -5505,7 +5501,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>7</v>
       </c>
@@ -5537,7 +5533,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>9</v>
       </c>
@@ -5569,7 +5565,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>13</v>
       </c>
@@ -5601,7 +5597,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -5633,7 +5629,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3</v>
       </c>
@@ -5665,7 +5661,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>4</v>
       </c>
@@ -5697,7 +5693,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>6</v>
       </c>
@@ -5729,7 +5725,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>11</v>
       </c>
@@ -5761,7 +5757,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>15</v>
       </c>
@@ -5793,7 +5789,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>16</v>
       </c>
@@ -5825,7 +5821,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>17</v>
       </c>
@@ -5857,7 +5853,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>8</v>
       </c>
@@ -5889,7 +5885,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>10</v>
       </c>
@@ -5921,7 +5917,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>12</v>
       </c>
@@ -5953,7 +5949,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>14</v>
       </c>
@@ -5994,27 +5990,26 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N1:N9"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6042,14 +6037,8 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>32</v>
       </c>
@@ -6077,14 +6066,11 @@
       <c r="L2" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="O2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>33</v>
       </c>
@@ -6112,14 +6098,11 @@
       <c r="L3" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="O3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>34</v>
       </c>
@@ -6130,7 +6113,7 @@
         <v>40</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>140</v>
+        <v>64</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>83</v>
@@ -6147,14 +6130,11 @@
       <c r="L4" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="N4" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="O4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>35</v>
       </c>
@@ -6182,14 +6162,11 @@
       <c r="L5" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="O5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>36</v>
       </c>
@@ -6217,14 +6194,11 @@
       <c r="L6" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="N6" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="O6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>37</v>
       </c>
@@ -6246,14 +6220,11 @@
       <c r="L7" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="N7" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="O7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>38</v>
       </c>
@@ -6272,14 +6243,11 @@
       <c r="L8" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="N8" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="O8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>39</v>
       </c>
@@ -6298,14 +6266,11 @@
       <c r="L9" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="N9" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="O9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>40</v>
       </c>
@@ -6324,14 +6289,11 @@
       <c r="L10" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="N10" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="O10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>41</v>
       </c>
@@ -6350,14 +6312,11 @@
       <c r="L11" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="N11" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="O11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>42</v>
       </c>
@@ -6376,14 +6335,11 @@
       <c r="L12" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="N12" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="O12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>43</v>
       </c>
@@ -6399,14 +6355,11 @@
       <c r="L13" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="N13" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="O13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>44</v>
       </c>
@@ -6419,14 +6372,11 @@
       <c r="L14" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="N14" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="O14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>45</v>
       </c>
@@ -6439,14 +6389,11 @@
       <c r="L15" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="N15" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="O15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
         <v>46</v>
       </c>
@@ -6459,14 +6406,11 @@
       <c r="L16" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="N16" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="O16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>47</v>
       </c>
@@ -6479,14 +6423,11 @@
       <c r="L17" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="N17" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="O17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>48</v>
       </c>
@@ -6499,14 +6440,11 @@
       <c r="L18" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="N18" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="O18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
         <v>49</v>
       </c>
@@ -6519,14 +6457,11 @@
       <c r="L19" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="N19" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="O19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
         <v>50</v>
       </c>
@@ -6539,14 +6474,11 @@
       <c r="L20" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="N20" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="O20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
         <v>51</v>
       </c>
@@ -6559,14 +6491,11 @@
       <c r="L21" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="N21" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="O21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>37</v>
       </c>
@@ -6576,73 +6505,66 @@
       <c r="L22" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="N22" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="O22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="F23" s="3" t="s">
         <v>88</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="N23" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="O23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="F24" s="3" t="s">
         <v>38</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="O24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
       <c r="O25">
         <f>SUM(O2:O24)</f>
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="N1:O24">
-    <sortCondition descending="1" ref="O24"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:P30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -6671,7 +6593,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>32</v>
       </c>
@@ -6699,14 +6621,11 @@
       <c r="L2" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>48</v>
       </c>
@@ -6734,14 +6653,11 @@
       <c r="L3" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>52</v>
       </c>
@@ -6769,14 +6685,11 @@
       <c r="L4" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="O4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>34</v>
       </c>
@@ -6804,14 +6717,11 @@
       <c r="L5" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="O5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="P5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>46</v>
       </c>
@@ -6839,14 +6749,11 @@
       <c r="L6" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="O6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="P6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>41</v>
       </c>
@@ -6865,14 +6772,11 @@
       <c r="L7" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="O7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="P7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>53</v>
       </c>
@@ -6891,14 +6795,11 @@
       <c r="L8" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="O8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="P8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>54</v>
       </c>
@@ -6917,14 +6818,11 @@
       <c r="L9" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="O9" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="P9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>55</v>
       </c>
@@ -6943,14 +6841,11 @@
       <c r="L10" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="O10" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="P10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>56</v>
       </c>
@@ -6969,14 +6864,11 @@
       <c r="L11" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="O11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="P11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>39</v>
       </c>
@@ -6992,14 +6884,11 @@
       <c r="L12" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="O12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>40</v>
       </c>
@@ -7015,14 +6904,11 @@
       <c r="L13" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="O13" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="P13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>36</v>
       </c>
@@ -7035,14 +6921,11 @@
       <c r="L14" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="O14" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="P14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>51</v>
       </c>
@@ -7055,14 +6938,11 @@
       <c r="L15" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="O15" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="P15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
         <v>57</v>
       </c>
@@ -7075,14 +6955,11 @@
       <c r="L16" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="O16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="P16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>58</v>
       </c>
@@ -7095,14 +6972,11 @@
       <c r="L17" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="O17" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="P17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>37</v>
       </c>
@@ -7115,151 +6989,115 @@
       <c r="L18" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="O18" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="P18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
         <v>44</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="O19" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="P19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
         <v>59</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="O20" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="P20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
         <v>60</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="O21" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="P21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>61</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="O22" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="P22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>62</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="O23" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="P23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
         <v>63</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="O24" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="P24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="L25" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="O25" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="L26" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="O26" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="P26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="L27" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="O27" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="P27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="L28" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="O28" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="P30">
-        <f>SUM(P2:P28)</f>
+      <c r="M28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="M30">
+        <f>SUM(M2:M28)</f>
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="O2:P28">
-    <sortCondition ref="P2:P28"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Revert "Revert "Revert "Yes""""
This reverts commit 57159e96fd159307308d8767f3a1b476010679e7.
</commit_message>
<xml_diff>
--- a/SUS_INTUI_WORD.xlsx
+++ b/SUS_INTUI_WORD.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marianne\Desktop\P8-Analyse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\test1\Documents\P8\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682AE9FC-79D2-4099-905A-5750131E54F9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11556" windowHeight="7596" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11550" windowHeight="7590" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SusHelix" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
     <sheet name="WordHelix" sheetId="5" r:id="rId7"/>
     <sheet name="WordHeadrush" sheetId="6" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="141">
   <si>
     <t>Helix</t>
   </si>
@@ -451,12 +452,15 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>Comprehensiv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -510,7 +514,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Procent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -533,7 +537,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="da-DK"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -570,7 +574,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="da-DK"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1326,7 +1330,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="da-DK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="449834784"/>
@@ -1385,7 +1389,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="da-DK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="449834128"/>
@@ -1427,7 +1431,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="da-DK"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1457,7 +1461,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="da-DK"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2066,9 +2070,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kontor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2106,7 +2110,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kontor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2212,7 +2216,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kontor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2361,20 +2365,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.21875" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2403,7 +2407,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2432,7 +2436,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2461,7 +2465,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2490,7 +2494,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2519,7 +2523,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2548,7 +2552,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2577,7 +2581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2606,7 +2610,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2635,7 +2639,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2664,7 +2668,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2693,7 +2697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13">
         <f>(((B2-1)+(5-B3)+(B4-1)+(5-B5)+(B6-1)+(5-B7)+(B8-1)+(5-B9)+(B10-1)+(5-B11))*2.5)</f>
         <v>60</v>
@@ -2737,16 +2741,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView topLeftCell="B7" workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -2778,7 +2782,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2811,7 +2815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2844,7 +2848,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2877,7 +2881,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2910,7 +2914,7 @@
         <v>2.375</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2943,7 +2947,7 @@
         <v>3.625</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2976,7 +2980,7 @@
         <v>2.125</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3009,7 +3013,7 @@
         <v>3.875</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3042,7 +3046,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3075,7 +3079,7 @@
         <v>3.375</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3108,7 +3112,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13">
         <f>(((B2-1)+(5-B3)+(B4-1)+(5-B5)+(B6-1)+(5-B7)+(B8-1)+(5-B9)+(B10-1)+(5-B11))*2.5)</f>
         <v>75</v>
@@ -3153,16 +3157,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J18" sqref="A1:J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3191,7 +3195,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3223,7 +3227,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3255,7 +3259,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3287,7 +3291,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3319,7 +3323,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3351,7 +3355,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3383,7 +3387,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3415,7 +3419,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3447,7 +3451,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3479,7 +3483,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3515,7 +3519,7 @@
         <v>3.375</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3547,7 +3551,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3579,7 +3583,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3611,7 +3615,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3643,7 +3647,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3675,7 +3679,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3707,7 +3711,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3739,7 +3743,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -3781,10 +3785,10 @@
       </c>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -3826,10 +3830,10 @@
       </c>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -3871,10 +3875,10 @@
       </c>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -3916,10 +3920,10 @@
       </c>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -3967,16 +3971,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J18" sqref="A1:J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -4005,7 +4009,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4037,7 +4041,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4069,7 +4073,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4104,7 +4108,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4136,7 +4140,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4168,7 +4172,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4203,7 +4207,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4235,7 +4239,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4270,7 +4274,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4305,7 +4309,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4341,7 +4345,7 @@
         <v>4.125</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4373,7 +4377,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4405,7 +4409,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4440,7 +4444,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4475,7 +4479,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4507,7 +4511,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4542,7 +4546,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4574,7 +4578,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -4616,10 +4620,10 @@
       </c>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -4661,10 +4665,10 @@
       </c>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -4706,10 +4710,10 @@
       </c>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -4751,10 +4755,10 @@
       </c>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -4802,16 +4806,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -4843,7 +4847,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -4875,7 +4879,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -4907,7 +4911,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>7</v>
       </c>
@@ -4939,7 +4943,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9</v>
       </c>
@@ -4971,7 +4975,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>13</v>
       </c>
@@ -5003,7 +5007,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -5035,7 +5039,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -5067,7 +5071,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -5099,7 +5103,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -5131,7 +5135,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
@@ -5163,7 +5167,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>15</v>
       </c>
@@ -5195,7 +5199,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>16</v>
       </c>
@@ -5227,7 +5231,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>17</v>
       </c>
@@ -5259,7 +5263,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>8</v>
       </c>
@@ -5291,7 +5295,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>10</v>
       </c>
@@ -5323,7 +5327,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>12</v>
       </c>
@@ -5355,7 +5359,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
@@ -5396,16 +5400,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5437,7 +5441,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -5469,7 +5473,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -5501,7 +5505,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>7</v>
       </c>
@@ -5533,7 +5537,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9</v>
       </c>
@@ -5565,7 +5569,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>13</v>
       </c>
@@ -5597,7 +5601,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -5629,7 +5633,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -5661,7 +5665,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -5693,7 +5697,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -5725,7 +5729,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
@@ -5757,7 +5761,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>15</v>
       </c>
@@ -5789,7 +5793,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>16</v>
       </c>
@@ -5821,7 +5825,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>17</v>
       </c>
@@ -5853,7 +5857,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>8</v>
       </c>
@@ -5885,7 +5889,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>10</v>
       </c>
@@ -5917,7 +5921,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>12</v>
       </c>
@@ -5949,7 +5953,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
@@ -5990,26 +5994,27 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="N9" sqref="N1:N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6037,8 +6042,14 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="N1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>32</v>
       </c>
@@ -6066,11 +6077,14 @@
       <c r="L2" s="2" t="s">
         <v>94</v>
       </c>
+      <c r="N2" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="O2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>33</v>
       </c>
@@ -6098,11 +6112,14 @@
       <c r="L3" s="2" t="s">
         <v>95</v>
       </c>
+      <c r="N3" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="O3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>34</v>
       </c>
@@ -6113,7 +6130,7 @@
         <v>40</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>64</v>
+        <v>140</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>83</v>
@@ -6130,11 +6147,14 @@
       <c r="L4" s="2" t="s">
         <v>96</v>
       </c>
+      <c r="N4" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="O4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>35</v>
       </c>
@@ -6162,11 +6182,14 @@
       <c r="L5" s="2" t="s">
         <v>97</v>
       </c>
+      <c r="N5" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="O5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>36</v>
       </c>
@@ -6194,11 +6217,14 @@
       <c r="L6" s="2" t="s">
         <v>98</v>
       </c>
+      <c r="N6" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="O6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>37</v>
       </c>
@@ -6220,11 +6246,14 @@
       <c r="L7" s="2" t="s">
         <v>99</v>
       </c>
+      <c r="N7" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="O7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>38</v>
       </c>
@@ -6243,11 +6272,14 @@
       <c r="L8" s="2" t="s">
         <v>100</v>
       </c>
+      <c r="N8" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="O8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>39</v>
       </c>
@@ -6266,11 +6298,14 @@
       <c r="L9" s="2" t="s">
         <v>101</v>
       </c>
+      <c r="N9" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="O9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>40</v>
       </c>
@@ -6289,11 +6324,14 @@
       <c r="L10" s="2" t="s">
         <v>102</v>
       </c>
+      <c r="N10" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="O10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>41</v>
       </c>
@@ -6312,11 +6350,14 @@
       <c r="L11" s="2" t="s">
         <v>103</v>
       </c>
+      <c r="N11" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="O11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>42</v>
       </c>
@@ -6335,11 +6376,14 @@
       <c r="L12" s="2" t="s">
         <v>104</v>
       </c>
+      <c r="N12" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="O12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>43</v>
       </c>
@@ -6355,11 +6399,14 @@
       <c r="L13" s="2" t="s">
         <v>105</v>
       </c>
+      <c r="N13" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="O13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>44</v>
       </c>
@@ -6372,11 +6419,14 @@
       <c r="L14" s="2" t="s">
         <v>106</v>
       </c>
+      <c r="N14" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="O14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>45</v>
       </c>
@@ -6389,11 +6439,14 @@
       <c r="L15" s="2" t="s">
         <v>107</v>
       </c>
+      <c r="N15" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="O15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>46</v>
       </c>
@@ -6406,11 +6459,14 @@
       <c r="L16" s="2" t="s">
         <v>108</v>
       </c>
+      <c r="N16" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="O16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>47</v>
       </c>
@@ -6423,11 +6479,14 @@
       <c r="L17" s="2" t="s">
         <v>109</v>
       </c>
+      <c r="N17" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="O17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>48</v>
       </c>
@@ -6440,11 +6499,14 @@
       <c r="L18" s="2" t="s">
         <v>110</v>
       </c>
+      <c r="N18" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="O18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>49</v>
       </c>
@@ -6457,11 +6519,14 @@
       <c r="L19" s="2" t="s">
         <v>111</v>
       </c>
+      <c r="N19" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="O19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>50</v>
       </c>
@@ -6474,11 +6539,14 @@
       <c r="L20" s="2" t="s">
         <v>112</v>
       </c>
+      <c r="N20" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="O20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>51</v>
       </c>
@@ -6491,11 +6559,14 @@
       <c r="L21" s="2" t="s">
         <v>113</v>
       </c>
+      <c r="N21" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="O21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>37</v>
       </c>
@@ -6505,66 +6576,73 @@
       <c r="L22" s="2" t="s">
         <v>119</v>
       </c>
+      <c r="N22" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="O22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F23" s="3" t="s">
         <v>88</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>114</v>
       </c>
+      <c r="N23" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="O23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F24" s="3" t="s">
         <v>38</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="O24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O25">
         <f>SUM(O2:O24)</f>
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="N1:O24">
+    <sortCondition descending="1" ref="O24"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -6593,7 +6671,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>32</v>
       </c>
@@ -6621,11 +6699,14 @@
       <c r="L2" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="M2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>48</v>
       </c>
@@ -6653,11 +6734,14 @@
       <c r="L3" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="M3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>52</v>
       </c>
@@ -6685,11 +6769,14 @@
       <c r="L4" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>34</v>
       </c>
@@ -6717,11 +6804,14 @@
       <c r="L5" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="M5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>46</v>
       </c>
@@ -6749,11 +6839,14 @@
       <c r="L6" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="M6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>41</v>
       </c>
@@ -6772,11 +6865,14 @@
       <c r="L7" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>53</v>
       </c>
@@ -6795,11 +6891,14 @@
       <c r="L8" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="M8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>54</v>
       </c>
@@ -6818,11 +6917,14 @@
       <c r="L9" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O9" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>55</v>
       </c>
@@ -6841,11 +6943,14 @@
       <c r="L10" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="M10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>56</v>
       </c>
@@ -6864,11 +6969,14 @@
       <c r="L11" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="M11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>39</v>
       </c>
@@ -6884,11 +6992,14 @@
       <c r="L12" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="M12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>40</v>
       </c>
@@ -6904,11 +7015,14 @@
       <c r="L13" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="M13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>36</v>
       </c>
@@ -6921,11 +7035,14 @@
       <c r="L14" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="M14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O14" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>51</v>
       </c>
@@ -6938,11 +7055,14 @@
       <c r="L15" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="M15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>57</v>
       </c>
@@ -6955,11 +7075,14 @@
       <c r="L16" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="M16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>58</v>
       </c>
@@ -6972,11 +7095,14 @@
       <c r="L17" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="M17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O17" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>37</v>
       </c>
@@ -6989,115 +7115,151 @@
       <c r="L18" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="M18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>44</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="M19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>59</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="M20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="P20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>60</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="M21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>61</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="M22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O22" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="P22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>62</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="M23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O23" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="P23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>63</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="M24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O24" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="P24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L25" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="M25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O25" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L26" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="M26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O26" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="P26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L27" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="M27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="P27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L28" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="M28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="M30">
-        <f>SUM(M2:M28)</f>
+      <c r="O28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="P28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="P30">
+        <f>SUM(P2:P28)</f>
         <v>40</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="O2:P28">
+    <sortCondition ref="P2:P28"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>